<commit_message>
🚀 Versión v4.12 estable | Flujo completo Control_ANS funcional: ✔️ Descarga y clasificación de evidencias por responsable ✔️ Detección automática de entorno (Empresa / Personal) ✔️ Actualización FENIX_ANS y repositorio de pedidos cerrados ✔️ Preparado para ejecución final con tkinter y Power BI
</commit_message>
<xml_diff>
--- a/data_clean/REPOSITORIO_PEDIDOS_CERRADOS.xlsx
+++ b/data_clean/REPOSITORIO_PEDIDOS_CERRADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,10 +612,8 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>054926309110740000</t>
-        </is>
+      <c r="M2" t="n">
+        <v>5.492630911074e+16</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -722,10 +720,8 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>055224007200130201</t>
-        </is>
+      <c r="M3" t="n">
+        <v>5.52240072001302e+16</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -832,10 +828,8 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>055224007200130301</t>
-        </is>
+      <c r="M4" t="n">
+        <v>5.52240072001303e+16</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -884,6 +878,676 @@
         </is>
       </c>
       <c r="X4" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>23087278</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ENERES</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ENERES</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>18/04/2024 09:10</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>45939.74375</v>
+      </c>
+      <c r="G5" t="n">
+        <v>71603529</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>GERMAN DE JESUS MARIN HENAO</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>4657981</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3207426955</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>CR 24 CL 57 B -13 (INTERIOR 302 )</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>055224007200130302</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>ALEGA</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>METROSUR Vin. Leg. Ref. Concentrada</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Urbano</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>45951.74375</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>15 días 17:51</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>23153422</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ENERES</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ENEDOM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10/07/2024 13:05</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>45944.56041666667</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1035861667</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>LIZANA PATRICIA BEDOYA MEJIA</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>3246410113</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>CR 1 ESTE CL 47 C -18</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>704021007300180000</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>ARTER</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Habilitación Viviendas Metrosur</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Urbano</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>45951.56041666667</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>13 días 13:27</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>23224950</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ENECNX</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ENECNX</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>09/10/2025 10:40</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>45939.44444444445</v>
+      </c>
+      <c r="G7" t="n">
+        <v>901761829</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>TAHOE LAQUE SAS TAHOE LAQUE SAS</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>3103589945</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>RURAL_114003250000000000_VEREDA_EL JARDIN</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>114003250000000000</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>ACREV</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Revisor Puntos de Conexión Metrosur</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" s="2" t="n">
+        <v>45946.44444444445</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>15 días 10:40</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23252866</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ENERES</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ENEDOM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>08/10/2025 15:54</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>45938.6625</v>
+      </c>
+      <c r="G8" t="n">
+        <v>98584619</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CALEB OBED RAMIREZ MUÑOZ</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>3002300945</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CR 34 E CL 31 -190 (INTERIOR 119 )</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>053324501001900119</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>AEJDO</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Habilitación Viviendas Metrosur</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Urbano</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <v>45946.6625</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>16 días 15:54</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>23332144</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ENENOR</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ENENOR</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>20/01/2025 09:02</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>45930.31180555555</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8355854</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>JUAN CARLOS LOPEZ MOLINA</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>9876543</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>RURAL_140004950000000049_PROV.PARCELACION VOLTA HO</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>ENVIGADO</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>140004950000000049</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>ALEGN</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Revisor Instalac. Regadas Oriente</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="R9" t="n">
+        <v>10</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <v>45945.31180555555</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>22 días 07:29</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>23499958</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ENEMRT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ENEMVI</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>29/07/2025 14:48</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>45894.37777777778</v>
+      </c>
+      <c r="G10" t="n">
+        <v>71590457</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO JARAMILLO MESA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>3113651861</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>RURAL_147014002000000000_147014002000000000</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>147014002000000000</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>AMRTR</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>MET-RMRT-Francisco J Dominguez</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
+        <v>10</v>
+      </c>
+      <c r="S10" s="2" t="n">
+        <v>45908.37777777778</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>48 días 09:04</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
         <is>
           <t>Ejecutado en Campo</t>
         </is>

</xml_diff>

<commit_message>
v4.13 estable | Flujo completo validado en entorno empresa: cálculo ANS y descarga Drive
</commit_message>
<xml_diff>
--- a/data_clean/REPOSITORIO_PEDIDOS_CERRADOS.xlsx
+++ b/data_clean/REPOSITORIO_PEDIDOS_CERRADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,16 @@
           <t>REPORTE_TECNICO</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>AREA_OPERATIVA</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>SUBZONA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -612,8 +622,10 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M2" t="n">
-        <v>5.492630911074e+16</v>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>054926309110740000</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -643,7 +655,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>17 días 09:36</t>
+          <t>18 días 09:36</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -666,6 +678,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -720,8 +734,10 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M3" t="n">
-        <v>5.52240072001302e+16</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>055224007200130201</t>
+        </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -751,7 +767,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>15 días 17:48</t>
+          <t>16 días 17:48</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -774,6 +790,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -828,8 +846,10 @@
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M4" t="n">
-        <v>5.52240072001303e+16</v>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>055224007200130301</t>
+        </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -859,7 +879,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>15 días 17:50</t>
+          <t>16 días 17:50</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -882,6 +902,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -969,7 +991,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>15 días 17:51</t>
+          <t>16 días 17:51</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -992,6 +1014,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1081,7 +1105,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>13 días 13:27</t>
+          <t>14 días 13:27</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1104,6 +1128,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1193,7 +1219,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>15 días 10:40</t>
+          <t>16 días 10:40</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1216,6 +1242,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1305,7 +1333,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>16 días 15:54</t>
+          <t>17 días 15:54</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1328,6 +1356,8 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1417,7 +1447,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>22 días 07:29</t>
+          <t>23 días 07:29</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1440,118 +1470,236 @@
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>23398679</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ENERES</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NUEVO</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ENEDOM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>27/03/2025 15:02</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>45924.42361111111</v>
+      </c>
+      <c r="G10" t="n">
+        <v>43874896</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>LUZ EDITH MONTOYA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>SIN DATOS</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>3107440550</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>RURAL_130023595050000002</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>GUARNE</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>130023595050000002</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>ARTER</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Habilitación Viviendas Oriente</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
+        <v>8</v>
+      </c>
+      <c r="S10" s="2" t="n">
+        <v>45936.42361111111</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>27 días 10:10</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Ejecutado en Campo</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>23499958</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>ENEMRT</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>NUEVO</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>ENEMVI</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>29/07/2025 14:48</t>
         </is>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F11" s="2" t="n">
         <v>45894.37777777778</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G11" t="n">
         <v>71590457</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>CARLOS ALBERTO JARAMILLO MESA</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>SIN DATOS</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J11" t="n">
         <v>3113651861</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>RURAL_147014002000000000_147014002000000000</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>MEDELLÍN</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>147014002000000000</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>Medellín</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>AMRTR</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>MET-RMRT-Francisco J Dominguez</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Rural</t>
         </is>
       </c>
-      <c r="R10" t="n">
+      <c r="R11" t="n">
         <v>10</v>
       </c>
-      <c r="S10" s="2" t="n">
+      <c r="S11" s="2" t="n">
         <v>45908.37777777778</v>
       </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>48 días 09:04</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>VENCIDO</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>VENCIDO</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>49 días 09:04</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t>CERRADO</t>
         </is>
       </c>
-      <c r="X10" t="inlineStr">
+      <c r="X11" t="inlineStr">
         <is>
           <t>Ejecutado en Campo</t>
         </is>
       </c>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>